<commit_message>
Cleanedup weapons/armour and added a new command to clean up invalid weapons.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Weapons/bows.xlsx
+++ b/resources/data-imports/Weapons/bows.xlsx
@@ -602,8 +602,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -686,7 +687,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -697,6 +698,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -893,13 +898,14 @@
   </sheetPr>
   <dimension ref="A1:BT60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V61" activeCellId="0" sqref="V61:Y61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L60" activeCellId="0" sqref="L2:L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="42.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="19.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="20.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="17.39"/>
@@ -1148,8 +1154,8 @@
       <c r="I2" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="L2" s="1" t="n">
-        <v>10</v>
+      <c r="L2" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>0</v>
@@ -1276,8 +1282,8 @@
       <c r="I3" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="L3" s="1" t="n">
-        <v>16</v>
+      <c r="L3" s="3" t="n">
+        <v>13</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>0</v>
@@ -1392,8 +1398,8 @@
       <c r="I4" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="L4" s="1" t="n">
-        <v>27</v>
+      <c r="L4" s="3" t="n">
+        <v>19</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>0</v>
@@ -1508,8 +1514,8 @@
       <c r="I5" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="L5" s="1" t="n">
-        <v>45</v>
+      <c r="L5" s="3" t="n">
+        <v>28</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>0</v>
@@ -1624,8 +1630,8 @@
       <c r="I6" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="L6" s="1" t="n">
-        <v>73</v>
+      <c r="L6" s="3" t="n">
+        <v>40</v>
       </c>
       <c r="M6" s="1" t="n">
         <v>0</v>
@@ -1740,8 +1746,8 @@
       <c r="I7" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="L7" s="1" t="n">
-        <v>121</v>
+      <c r="L7" s="3" t="n">
+        <v>59</v>
       </c>
       <c r="M7" s="1" t="n">
         <v>0</v>
@@ -1856,8 +1862,8 @@
       <c r="I8" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="L8" s="1" t="n">
-        <v>199</v>
+      <c r="L8" s="3" t="n">
+        <v>87</v>
       </c>
       <c r="O8" s="1" t="n">
         <v>0</v>
@@ -1966,8 +1972,8 @@
       <c r="I9" s="1" t="n">
         <v>126</v>
       </c>
-      <c r="L9" s="1" t="n">
-        <v>328</v>
+      <c r="L9" s="3" t="n">
+        <v>127</v>
       </c>
       <c r="O9" s="1" t="n">
         <v>0</v>
@@ -2073,8 +2079,8 @@
       <c r="I10" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="L10" s="1" t="n">
-        <v>539</v>
+      <c r="L10" s="3" t="n">
+        <v>186</v>
       </c>
       <c r="O10" s="1" t="n">
         <v>0</v>
@@ -2180,8 +2186,8 @@
       <c r="I11" s="1" t="n">
         <v>160</v>
       </c>
-      <c r="L11" s="1" t="n">
-        <v>888</v>
+      <c r="L11" s="3" t="n">
+        <v>273</v>
       </c>
       <c r="O11" s="1" t="n">
         <v>0</v>
@@ -2287,8 +2293,8 @@
       <c r="I12" s="1" t="n">
         <v>177</v>
       </c>
-      <c r="L12" s="1" t="n">
-        <v>1462</v>
+      <c r="L12" s="3" t="n">
+        <v>399</v>
       </c>
       <c r="O12" s="1" t="n">
         <v>0</v>
@@ -2394,8 +2400,8 @@
       <c r="I13" s="1" t="n">
         <v>195</v>
       </c>
-      <c r="L13" s="1" t="n">
-        <v>2406</v>
+      <c r="L13" s="3" t="n">
+        <v>585</v>
       </c>
       <c r="O13" s="1" t="n">
         <v>0</v>
@@ -2501,8 +2507,8 @@
       <c r="I14" s="1" t="n">
         <v>212</v>
       </c>
-      <c r="L14" s="1" t="n">
-        <v>3961</v>
+      <c r="L14" s="3" t="n">
+        <v>856</v>
       </c>
       <c r="O14" s="1" t="n">
         <v>0</v>
@@ -2608,8 +2614,8 @@
       <c r="I15" s="1" t="n">
         <v>229</v>
       </c>
-      <c r="L15" s="1" t="n">
-        <v>6521</v>
+      <c r="L15" s="3" t="n">
+        <v>1254</v>
       </c>
       <c r="O15" s="1" t="n">
         <v>0</v>
@@ -2715,8 +2721,8 @@
       <c r="I16" s="1" t="n">
         <v>246</v>
       </c>
-      <c r="L16" s="1" t="n">
-        <v>10736</v>
+      <c r="L16" s="3" t="n">
+        <v>1837</v>
       </c>
       <c r="O16" s="1" t="n">
         <v>0</v>
@@ -2822,8 +2828,8 @@
       <c r="I17" s="1" t="n">
         <v>263</v>
       </c>
-      <c r="L17" s="1" t="n">
-        <v>17673</v>
+      <c r="L17" s="3" t="n">
+        <v>2691</v>
       </c>
       <c r="O17" s="1" t="n">
         <v>0</v>
@@ -2929,8 +2935,8 @@
       <c r="I18" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="L18" s="1" t="n">
-        <v>29094</v>
+      <c r="L18" s="3" t="n">
+        <v>3941</v>
       </c>
       <c r="O18" s="1" t="n">
         <v>0</v>
@@ -3036,8 +3042,8 @@
       <c r="I19" s="1" t="n">
         <v>297</v>
       </c>
-      <c r="L19" s="1" t="n">
-        <v>47896</v>
+      <c r="L19" s="3" t="n">
+        <v>5772</v>
       </c>
       <c r="O19" s="1" t="n">
         <v>0</v>
@@ -3143,8 +3149,8 @@
       <c r="I20" s="1" t="n">
         <v>314</v>
       </c>
-      <c r="L20" s="1" t="n">
-        <v>78847</v>
+      <c r="L20" s="3" t="n">
+        <v>8454</v>
       </c>
       <c r="O20" s="1" t="n">
         <v>0</v>
@@ -3250,8 +3256,8 @@
       <c r="I21" s="1" t="n">
         <v>332</v>
       </c>
-      <c r="L21" s="1" t="n">
-        <v>129799</v>
+      <c r="L21" s="3" t="n">
+        <v>12382</v>
       </c>
       <c r="O21" s="1" t="n">
         <v>0</v>
@@ -3357,8 +3363,8 @@
       <c r="I22" s="1" t="n">
         <v>349</v>
       </c>
-      <c r="L22" s="1" t="n">
-        <v>213678</v>
+      <c r="L22" s="3" t="n">
+        <v>18135</v>
       </c>
       <c r="O22" s="1" t="n">
         <v>0</v>
@@ -3464,8 +3470,8 @@
       <c r="I23" s="1" t="n">
         <v>366</v>
       </c>
-      <c r="L23" s="1" t="n">
-        <v>351761</v>
+      <c r="L23" s="3" t="n">
+        <v>26561</v>
       </c>
       <c r="O23" s="1" t="n">
         <v>0</v>
@@ -3571,8 +3577,8 @@
       <c r="I24" s="1" t="n">
         <v>383</v>
       </c>
-      <c r="L24" s="1" t="n">
-        <v>579076</v>
+      <c r="L24" s="3" t="n">
+        <v>38902</v>
       </c>
       <c r="O24" s="1" t="n">
         <v>0</v>
@@ -3678,8 +3684,8 @@
       <c r="I25" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="L25" s="1" t="n">
-        <v>953286</v>
+      <c r="L25" s="3" t="n">
+        <v>56977</v>
       </c>
       <c r="O25" s="1" t="n">
         <v>0</v>
@@ -3785,8 +3791,8 @@
       <c r="I26" s="1" t="n">
         <v>417</v>
       </c>
-      <c r="L26" s="1" t="n">
-        <v>1569320</v>
+      <c r="L26" s="3" t="n">
+        <v>83451</v>
       </c>
       <c r="O26" s="1" t="n">
         <v>0</v>
@@ -3892,8 +3898,8 @@
       <c r="I27" s="1" t="n">
         <v>434</v>
       </c>
-      <c r="L27" s="1" t="n">
-        <v>2583446</v>
+      <c r="L27" s="3" t="n">
+        <v>122226</v>
       </c>
       <c r="O27" s="1" t="n">
         <v>0</v>
@@ -3999,8 +4005,8 @@
       <c r="I28" s="1" t="n">
         <v>452</v>
       </c>
-      <c r="L28" s="1" t="n">
-        <v>4252921</v>
+      <c r="L28" s="3" t="n">
+        <v>179017</v>
       </c>
       <c r="O28" s="1" t="n">
         <v>0</v>
@@ -4106,8 +4112,8 @@
       <c r="I29" s="1" t="n">
         <v>469</v>
       </c>
-      <c r="L29" s="1" t="n">
-        <v>7001245</v>
+      <c r="L29" s="3" t="n">
+        <v>262195</v>
       </c>
       <c r="O29" s="1" t="n">
         <v>0</v>
@@ -4213,8 +4219,8 @@
       <c r="I30" s="1" t="n">
         <v>486</v>
       </c>
-      <c r="L30" s="1" t="n">
-        <v>11525593</v>
+      <c r="L30" s="3" t="n">
+        <v>384022</v>
       </c>
       <c r="O30" s="1" t="n">
         <v>0</v>
@@ -4320,8 +4326,8 @@
       <c r="I31" s="1" t="n">
         <v>503</v>
       </c>
-      <c r="L31" s="1" t="n">
-        <v>18973666</v>
+      <c r="L31" s="3" t="n">
+        <v>562454</v>
       </c>
       <c r="O31" s="1" t="n">
         <v>0</v>
@@ -4427,8 +4433,8 @@
       <c r="I32" s="1" t="n">
         <v>520</v>
       </c>
-      <c r="L32" s="1" t="n">
-        <v>31234836</v>
+      <c r="L32" s="3" t="n">
+        <v>823793</v>
       </c>
       <c r="O32" s="1" t="n">
         <v>0</v>
@@ -4534,8 +4540,8 @@
       <c r="I33" s="1" t="n">
         <v>537</v>
       </c>
-      <c r="L33" s="1" t="n">
-        <v>51419423</v>
+      <c r="L33" s="3" t="n">
+        <v>1206561</v>
       </c>
       <c r="M33" s="1" t="n">
         <v>0</v>
@@ -4650,8 +4656,8 @@
       <c r="I34" s="1" t="n">
         <v>554</v>
       </c>
-      <c r="L34" s="1" t="n">
-        <v>84647702</v>
+      <c r="L34" s="3" t="n">
+        <v>1767179</v>
       </c>
       <c r="M34" s="1" t="n">
         <v>0</v>
@@ -4766,8 +4772,8 @@
       <c r="I35" s="1" t="n">
         <v>572</v>
       </c>
-      <c r="L35" s="1" t="n">
-        <v>139348772</v>
+      <c r="L35" s="3" t="n">
+        <v>2588282</v>
       </c>
       <c r="O35" s="1" t="n">
         <v>0</v>
@@ -4876,8 +4882,8 @@
       <c r="I36" s="1" t="n">
         <v>589</v>
       </c>
-      <c r="L36" s="1" t="n">
-        <v>229398789</v>
+      <c r="L36" s="3" t="n">
+        <v>3790904</v>
       </c>
       <c r="O36" s="1" t="n">
         <v>0</v>
@@ -4986,8 +4992,8 @@
       <c r="I37" s="1" t="n">
         <v>606</v>
       </c>
-      <c r="L37" s="1" t="n">
-        <v>377640962</v>
+      <c r="L37" s="3" t="n">
+        <v>5552314</v>
       </c>
       <c r="O37" s="1" t="n">
         <v>0</v>
@@ -5096,8 +5102,8 @@
       <c r="I38" s="1" t="n">
         <v>623</v>
       </c>
-      <c r="L38" s="1" t="n">
-        <v>621680248</v>
+      <c r="L38" s="3" t="n">
+        <v>8132146</v>
       </c>
       <c r="M38" s="1" t="n">
         <v>0</v>
@@ -5212,8 +5218,8 @@
       <c r="I39" s="1" t="n">
         <v>640</v>
       </c>
-      <c r="L39" s="1" t="n">
-        <v>1023422695</v>
+      <c r="L39" s="3" t="n">
+        <v>11910675</v>
       </c>
       <c r="O39" s="1" t="n">
         <v>0</v>
@@ -5322,8 +5328,8 @@
       <c r="I40" s="1" t="n">
         <v>657</v>
       </c>
-      <c r="L40" s="1" t="n">
-        <v>1684779299</v>
+      <c r="L40" s="3" t="n">
+        <v>17444863</v>
       </c>
       <c r="M40" s="1" t="n">
         <v>0</v>
@@ -5438,8 +5444,8 @@
       <c r="I41" s="1" t="n">
         <v>674</v>
       </c>
-      <c r="L41" s="1" t="n">
-        <v>2000000000</v>
+      <c r="L41" s="3" t="n">
+        <v>25550461</v>
       </c>
       <c r="O41" s="1" t="n">
         <v>0</v>
@@ -5548,8 +5554,8 @@
       <c r="I42" s="1" t="n">
         <v>692</v>
       </c>
-      <c r="L42" s="1" t="n">
-        <v>4565821891</v>
+      <c r="L42" s="3" t="n">
+        <v>37422253</v>
       </c>
       <c r="O42" s="1" t="n">
         <v>0</v>
@@ -5658,8 +5664,8 @@
       <c r="I43" s="1" t="n">
         <v>709</v>
       </c>
-      <c r="L43" s="1" t="n">
-        <v>7516349053</v>
+      <c r="L43" s="3" t="n">
+        <v>54810166</v>
       </c>
       <c r="O43" s="1" t="n">
         <v>0</v>
@@ -5768,8 +5774,8 @@
       <c r="I44" s="1" t="n">
         <v>726</v>
       </c>
-      <c r="L44" s="1" t="n">
-        <v>12373567002</v>
+      <c r="L44" s="3" t="n">
+        <v>80277216</v>
       </c>
       <c r="O44" s="1" t="n">
         <v>0</v>
@@ -5878,8 +5884,8 @@
       <c r="I45" s="1" t="n">
         <v>743</v>
       </c>
-      <c r="L45" s="1" t="n">
-        <v>20369618184</v>
+      <c r="L45" s="3" t="n">
+        <v>117577302</v>
       </c>
       <c r="O45" s="1" t="n">
         <v>0</v>
@@ -5988,8 +5994,8 @@
       <c r="I46" s="1" t="n">
         <v>760</v>
       </c>
-      <c r="L46" s="1" t="n">
-        <v>33532880608</v>
+      <c r="L46" s="3" t="n">
+        <v>172208537</v>
       </c>
       <c r="O46" s="1" t="n">
         <v>0</v>
@@ -6098,8 +6104,8 @@
       <c r="I47" s="1" t="n">
         <v>777</v>
       </c>
-      <c r="L47" s="1" t="n">
-        <v>55202511489</v>
+      <c r="L47" s="3" t="n">
+        <v>252223684</v>
       </c>
       <c r="O47" s="1" t="n">
         <v>0</v>
@@ -6208,8 +6214,8 @@
       <c r="I48" s="1" t="n">
         <v>794</v>
       </c>
-      <c r="L48" s="1" t="n">
-        <v>90875499493</v>
+      <c r="L48" s="3" t="n">
+        <v>369417149</v>
       </c>
       <c r="O48" s="1" t="n">
         <v>0</v>
@@ -6318,8 +6324,8 @@
       <c r="I49" s="1" t="n">
         <v>811</v>
       </c>
-      <c r="L49" s="1" t="n">
-        <v>149601099396</v>
+      <c r="L49" s="3" t="n">
+        <v>541063502</v>
       </c>
       <c r="O49" s="1" t="n">
         <v>0</v>
@@ -6431,8 +6437,8 @@
       <c r="I50" s="1" t="n">
         <v>829</v>
       </c>
-      <c r="L50" s="1" t="n">
-        <v>246276378840</v>
+      <c r="L50" s="3" t="n">
+        <v>792463789</v>
       </c>
       <c r="O50" s="1" t="n">
         <v>0</v>
@@ -6541,8 +6547,8 @@
       <c r="I51" s="1" t="n">
         <v>846</v>
       </c>
-      <c r="L51" s="1" t="n">
-        <v>405425194197</v>
+      <c r="L51" s="3" t="n">
+        <v>1160674956</v>
       </c>
       <c r="O51" s="1" t="n">
         <v>0</v>
@@ -6651,8 +6657,8 @@
       <c r="I52" s="1" t="n">
         <v>863</v>
       </c>
-      <c r="L52" s="1" t="n">
-        <v>667419217644</v>
+      <c r="L52" s="3" t="n">
+        <v>1699972128</v>
       </c>
       <c r="O52" s="1" t="n">
         <v>0</v>
@@ -6761,8 +6767,8 @@
       <c r="I53" s="1" t="n">
         <v>880</v>
       </c>
-      <c r="L53" s="1" t="n">
-        <v>1098719118734</v>
+      <c r="L53" s="3" t="n">
+        <v>2000000000</v>
       </c>
       <c r="O53" s="1" t="n">
         <v>0</v>
@@ -6874,8 +6880,8 @@
       <c r="K54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L54" s="1" t="n">
-        <v>1808733806216</v>
+      <c r="L54" s="3" t="n">
+        <v>3646734750</v>
       </c>
       <c r="O54" s="1" t="n">
         <v>0</v>
@@ -6984,8 +6990,8 @@
       <c r="I55" s="1" t="n">
         <v>914</v>
       </c>
-      <c r="L55" s="1" t="n">
-        <v>2977574455534</v>
+      <c r="L55" s="3" t="n">
+        <v>5341157231</v>
       </c>
       <c r="O55" s="1" t="n">
         <v>0</v>
@@ -7097,8 +7103,8 @@
       <c r="K56" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L56" s="1" t="n">
-        <v>4901743754542</v>
+      <c r="L56" s="3" t="n">
+        <v>7822877869</v>
       </c>
       <c r="O56" s="1" t="n">
         <v>0</v>
@@ -7210,8 +7216,8 @@
       <c r="K57" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L57" s="1" t="n">
-        <v>8069350470997</v>
+      <c r="L57" s="3" t="n">
+        <v>11457707664</v>
       </c>
       <c r="O57" s="1" t="n">
         <v>0</v>
@@ -7323,8 +7329,8 @@
       <c r="K58" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L58" s="1" t="n">
-        <v>13283929206508</v>
+      <c r="L58" s="3" t="n">
+        <v>16781428411</v>
       </c>
       <c r="O58" s="1" t="n">
         <v>0</v>
@@ -7436,8 +7442,8 @@
       <c r="K59" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L59" s="1" t="n">
-        <v>21868274999055</v>
+      <c r="L59" s="3" t="n">
+        <v>24578768089</v>
       </c>
       <c r="O59" s="1" t="n">
         <v>0</v>
@@ -7549,8 +7555,8 @@
       <c r="K60" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L60" s="1" t="n">
-        <v>36000000000000</v>
+      <c r="L60" s="3" t="n">
+        <v>35999071473</v>
       </c>
       <c r="O60" s="1" t="n">
         <v>0</v>

</xml_diff>